<commit_message>
Revert "Merge branch 'main' of https://github.com/DvaImi/Fantasy"
This reverts commit 9543e5d6c9371a4ce722012303483d15f9c0b6ed, reversing
changes made to 94d497f34dd97b01acf79a0a2afda64113b098d6.
</commit_message>
<xml_diff>
--- a/examples/Config/Excel/Server/MachineConfig.xlsx
+++ b/examples/Config/Excel/Server/MachineConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sining/Code/Git/Fantasy/Examples/Config/Excel/Server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0C31F7-D1CF-5744-82F4-318C79049089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F5E94D-F2D6-C543-9882-02121D762DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-900" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -139,6 +139,9 @@
   <si>
     <t>uint</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>127.0.0.1</t>
   </si>
   <si>
     <t>127.0.0.1</t>
@@ -573,7 +576,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -690,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'main' of https://github.com/DvaImi/Fantasy""
This reverts commit c799ec7ce1e04b9399b1741b03fb3cb11c07cb18.
</commit_message>
<xml_diff>
--- a/examples/Config/Excel/Server/MachineConfig.xlsx
+++ b/examples/Config/Excel/Server/MachineConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sining/Code/Git/Fantasy/Examples/Config/Excel/Server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F5E94D-F2D6-C543-9882-02121D762DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0C31F7-D1CF-5744-82F4-318C79049089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-900" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -139,9 +139,6 @@
   <si>
     <t>uint</t>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>127.0.0.1</t>
   </si>
   <si>
     <t>127.0.0.1</t>
@@ -576,7 +573,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -693,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>17</v>

</xml_diff>